<commit_message>
add HkmcVehicleInputAdap_SignalMatrix_V3 and Update HkmcVehicleInputAdap's Arxml
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V2.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veoneer.sharepoint.com/sites/KHTHKMCBN7FCAProject/Shared Documents/SOS and MVS4/01_Engineering/03_SW and FD/ApplicationSoftware/FeatureSignalMatrixs/HkmcVehicleInpAdap/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R2\02_SignalMatrix\HkmcVehicleInpAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D8C1467A-F4A0-450B-BB55-EDD6A2EFD8E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CF304AA0-E19A-4F26-800F-F9DDC1A2B287}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB36A388-A68B-49D4-A80F-972C60B6A3C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="261">
   <si>
     <t>Change Log</t>
   </si>
@@ -284,16 +284,6 @@
     <t>Input</t>
   </si>
   <si>
-    <t>Cx0_CruiseSS_IdlePosition
-Cx1_CruiseSS_Plus
-Cx2_CruiseSS_Minus
-Cx3_CruiseSS_Time_Gap
-Cx4_CruiseSS_Cancel_Pause
-Cx5_CruiseSS_Reserved
-Cx6_CruiseSS_Reserved
-Cx7_CruiseSS_Reserved</t>
-  </si>
-  <si>
     <t>4 Signals has been removed from HSCAN message CLU19 in new DBC</t>
   </si>
   <si>
@@ -323,13 +313,6 @@
     <t>BitLenght : 9 ; Factor : 0.5 ; Displayed vehicle speed</t>
   </si>
   <si>
-    <t>CF_Clu_SPEED_UNIT</t>
-  </si>
-  <si>
-    <t>Cx0_SpeedU_kmperh
-Cx1_SpeedU_MPH</t>
-  </si>
-  <si>
     <t>CF_Clu_AliveCnt1</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -346,16 +329,6 @@
   <si>
     <t>CF_AVN_FCANValueSet</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_FCANVS_Default
-Cx1_FCANVS_Off
-Cx2_FCANVS_Warning
-Cx3_FCANVS_Assist
-Cx4_FCANVS_Reserved
-Cx5_FCANVS_Reserved
-Cx6_FCANVS_Reserved
-Cx7_FCANVS_Invalid</t>
   </si>
   <si>
     <t>1 Signals has been removed from HSCAN message CLU19 in new DBC</t>
@@ -367,15 +340,6 @@
   <si>
     <t>Cx0_CluUSMR_Default
 Cx1_CluUSMR_Reset</t>
-  </si>
-  <si>
-    <t>CF_AVN_HDA_NValueSet</t>
-  </si>
-  <si>
-    <t>Cx0_HDANVS_Default
-Cx1_HDANVS_Function_Off
-Cx2_HDANVS_Function_On
-Cx3_HDANVS_Invalid</t>
   </si>
   <si>
     <t>New added signal in HSCAN message CLU19</t>
@@ -390,19 +354,6 @@
 Cx3_NSCCCNVS_Invalid</t>
   </si>
   <si>
-    <t>CF_AVN_WarningTimingNValueSet</t>
-  </si>
-  <si>
-    <t>Cx0_WarnTNVS_Default
-Cx1_WarnTNVS_Late
-Cx2_WarnTNVS_Normal
-Cx3_WarnTNVS_Reserved
-Cx4_WarnTNVS_Reserved
-Cx5_WarnTNVS_Reserved
-Cx6_WarnTNVS_Reserved
-Cx7_WarnTNVS_Invalid</t>
-  </si>
-  <si>
     <t>CF_AVN_LVDANValueSet</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -413,19 +364,6 @@
 Cx3_LVDANLVS_Invalid</t>
   </si>
   <si>
-    <t>CF_AVN_LkaModeNValueSet</t>
-  </si>
-  <si>
-    <t>Cx0_LkaMNVS_Default
-Cx1_LkaMNVS_LDW_mode
-Cx2_LkaMNVS_LKA
-Cx3_LkaMNVS_Reserved
-Cx4_LkaMNVS_LDW_only_ON
-Cx5_LkaMNVS_LDW_only_OFF
-Cx6_LkaMNVS_LDW_LKA_OFF
-Cx7_LkaMNVS_Invalid</t>
-  </si>
-  <si>
     <t>CF_AVN_HBANValueSet</t>
   </si>
   <si>
@@ -464,15 +402,8 @@
     <t xml:space="preserve">The human driver input torque on the steering column as measured by the MDPS torque and angle sensor. </t>
   </si>
   <si>
-    <t>5 Signals has been removed from HSCAN message MDPS12 in new DBC</t>
-  </si>
-  <si>
     <t>CF_Mdps_ToiUnavail</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_TU_Available
-Cx1_TU_Unavailable</t>
   </si>
   <si>
     <t>CF_Mdps_ToiActive</t>
@@ -506,9 +437,6 @@
     <t>This is a counter (counts continuously from 0 to its maximum bit count and back to 0 again), that can be used for checking the internal logic of the LKA controller.</t>
   </si>
   <si>
-    <t>CF_Mdps12_CRC</t>
-  </si>
-  <si>
     <t>BitLenght : 8; Factor: 1; CYCLIC REDUNDANCY CHECK</t>
   </si>
   <si>
@@ -521,16 +449,6 @@
   <si>
     <t>CF_Gway_IGNSw</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_IGNS_KeyOff
-Cx1_IGNS_KeyIn
-Cx2_IGNS_ACC
-Cx3_IGNS_IGN
-Cx4_IGNS_Start
-Cx5_IGNS_Reserved
-Cx6_IGNS_Reserved
-Cx7_IGNS_BCANSignalTimeOut</t>
   </si>
   <si>
     <t>CF_Gway_DrvDrSw</t>
@@ -606,19 +524,6 @@
 Cx1_WiperAS_On</t>
   </si>
   <si>
-    <t>CF_Gway_RainSnsState</t>
-  </si>
-  <si>
-    <t>Cx0_RainSS_OFF
-Cx1_RainSS_Rain_Detected
-Cx2_RainSS_Low
-Cx3_RainSS_High
-Cx4_RainSS_Fault1
-Cx5_RainSS_Fault2
-Cx6_RainSS_Fault3
-Cx7_RainSS_Reserved</t>
-  </si>
-  <si>
     <t>New added signal in HSCAN message CGW1</t>
   </si>
   <si>
@@ -714,9 +619,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2 Signals has been removed from CAN FD message CLU_01_20ms in new DBC</t>
-  </si>
-  <si>
     <t>CLU_AlvCnt1Val</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -732,29 +634,7 @@
     <t>CLU_SpdUnitTyp</t>
   </si>
   <si>
-    <t>CLU_SWRCCrsMainSwSta</t>
-  </si>
-  <si>
-    <t>Cx0_SWRCCMSS_off
-Cx1_SWRCCMSS_Key_On
-Cx2_SWRCCMSS_Reserved
-Cx3_SWRCCMSS_Invalid</t>
-  </si>
-  <si>
     <t>New added signal in CANFD message CLU_01_20ms</t>
-  </si>
-  <si>
-    <t>CLU_SWRCCrsSwSta</t>
-  </si>
-  <si>
-    <t>Cx0_SWRCCSS_Idle_Position
-Cx1_SWRCCSS_Plus
-Cx2_SWRCCSS_Minus
-Cx3_SWRCCSS_Headway
-Cx4_SWRCCSS_Cancel_Pause
-Cx5_SWRCCSS_Reserved
-Cx6_SWRCCSS_Reserved
-Cx7_SWRCCSS_Reserved</t>
   </si>
   <si>
     <t>CLU_SWRCLFASwSta</t>
@@ -767,21 +647,8 @@
 Cx3_SWRCLFASS_Invalid</t>
   </si>
   <si>
-    <t>CLU_SWRCSldMainSwSta</t>
-  </si>
-  <si>
-    <t>Cx0_SWRCSMSS_Off
-Cx1_SWRCSMSS_Key_On
-Cx2_SWRCSMSS_Reserved
-Cx3_SWRCSMSS_Invalid</t>
-  </si>
-  <si>
     <t>CLU_DisSpdVal</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BitLength:10, Factor : 0.5,CLU_DisplaySpeedValue
-Cx3FF : Error</t>
   </si>
   <si>
     <t>HSYS_CLU_05_00ms</t>
@@ -800,9 +667,6 @@
 Cx7_USMFca1stWSR_Invalid</t>
   </si>
   <si>
-    <t>3 Signals has been removed from CAN FD message CLU_05_00ms in new DBC</t>
-  </si>
-  <si>
     <t>USM_StaRst1Req</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -937,9 +801,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>3 Signals has been removed from CAN FD message CLU_13_00ms in new DBC</t>
-  </si>
-  <si>
     <t>CLU_AlvCnt13Val</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -970,27 +831,9 @@
 Cx3_AdasHbaSR_Invalid</t>
   </si>
   <si>
-    <t>USM_AdasDAWModNewSetReq</t>
-  </si>
-  <si>
-    <t>Cx0_AdasDAWMNSR_Default
-Cx1_AdasDAWMNSR_Off
-Cx2_AdasDAWMNSR_On
-Cx3_AdasDAWMNSR_Invalid</t>
-  </si>
-  <si>
     <t>New added signal in CAN FD message CLU_13_00ms</t>
   </si>
   <si>
-    <t>CLU_AdasDAWResetReq</t>
-  </si>
-  <si>
-    <t>Cx0_AdasDAWRR_Default
-Cx1_AdasDAWRR_ResetReq
-Cx2_AdasDAWRR_Reserved
-Cx3_AdasDAWRR_Invalid</t>
-  </si>
-  <si>
     <t>HSYS_MDPS_01_10ms</t>
   </si>
   <si>
@@ -1000,9 +843,6 @@
   <si>
     <t>BitLength:16, Factor : 1, MDPS_CyclicRedundancyCheck1Value ##2G##MDPS - MDPS11 - CF_Mdps_Chksum</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 Signals has been removed from CAN FD message MDPS_01_10ms in new DBC</t>
   </si>
   <si>
     <t>MDPS_AlvCnt1Val</t>
@@ -1107,7 +947,254 @@
     <t>HSYS_CLU_04_00ms</t>
   </si>
   <si>
-    <t>USM_AdasISLASetReq</t>
+    <t>CAN message added for ISLA adaptor</t>
+  </si>
+  <si>
+    <t>HkmcVehicleInput SWC/VIPCDD SWC</t>
+  </si>
+  <si>
+    <t>VIPCDD SWC</t>
+  </si>
+  <si>
+    <t>Port Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HVIA_MDPS</t>
+  </si>
+  <si>
+    <t>HVIA_CGW</t>
+  </si>
+  <si>
+    <t>HkmcVehicleInputAdap</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TopLevelCompostion/HkmcVehicleInput SWC</t>
+  </si>
+  <si>
+    <t>HkmcVehicleInput SWC</t>
+  </si>
+  <si>
+    <t>HSYS_CLU11</t>
+  </si>
+  <si>
+    <t>HSYS_CLU19</t>
+  </si>
+  <si>
+    <t>HSYS_MDPS12</t>
+  </si>
+  <si>
+    <t>HSYS_CGW1</t>
+  </si>
+  <si>
+    <t>HSYS_BCM_08_200ms</t>
+  </si>
+  <si>
+    <t>TopLevelCompostion</t>
+  </si>
+  <si>
+    <t>Cx0_ISLAOSR_Default
+Cx1_ISLAOSR_10kph_5mph
+Cx2_ISLAOSR_5kph_3mph
+Cx3_ISLAOSR_0
+Cx4_ISLAOSR_5kph_3mph
+Cx5_ISLAOSR_10kph_5mph
+Cx6_ISLAOSR_Reserved
+Cx7_ISLAOSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_CruiseSS_IdlePosition
+Cx1_CruiseSS_Plus
+Cx2_CruiseSS_Minus
+Cx3_CruiseSS_Time_Gap
+Cx4_CruiseSS_Cancel_Pause
+Cx5_CruiseSS_Reserved
+Cx6_CruiseSS_Reserved
+Cx7_CruiseSS_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_Clu_SPEED_UNIT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SpeedU_kmperh
+Cx1_SpeedU_MPH</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_FCANVS_Default
+Cx1_FCANVS_Off
+Cx2_FCANVS_Warning
+Cx3_FCANVS_Assist
+Cx4_FCANVS_Reserved
+Cx5_FCANVS_Reserved
+Cx6_FCANVS_Reserved
+Cx7_FCANVS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_AVN_HDA_NValueSet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_HDANVS_Default
+Cx1_HDANVS_Function_Off
+Cx2_HDANVS_Function_On
+Cx3_HDANVS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_AVN_WarningTimingNValueSet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_WarnTNVS_Default
+Cx1_WarnTNVS_Late
+Cx2_WarnTNVS_Normal
+Cx3_WarnTNVS_Reserved
+Cx4_WarnTNVS_Reserved
+Cx5_WarnTNVS_Reserved
+Cx6_WarnTNVS_Reserved
+Cx7_WarnTNVS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_AVN_LkaModeNValueSet</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaMNVS_Default
+Cx1_LkaMNVS_LDW_mode
+Cx2_LkaMNVS_LKA
+Cx3_LkaMNVS_Reserved
+Cx4_LkaMNVS_LDW_only_ON
+Cx5_LkaMNVS_LDW_only_OFF
+Cx6_LkaMNVS_LDW_LKA_OFF
+Cx7_LkaMNVS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 Signals has been removed from HSCAN message MDPS12 in new DBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_Mdps12_CRC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_IGNS_KeyOff
+Cx1_IGNS_KeyIn
+Cx2_IGNS_ACC
+Cx3_IGNS_IGN
+Cx4_IGNS_Start
+Cx5_IGNS_Reserved
+Cx6_IGNS_Reserved
+Cx7_IGNS_BCANSignalTimeOut</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF_Gway_RainSnsState</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_RainSS_OFF
+Cx1_RainSS_Rain_Detected
+Cx2_RainSS_Low
+Cx3_RainSS_High
+Cx4_RainSS_Fault1
+Cx5_RainSS_Fault2
+Cx6_RainSS_Fault3
+Cx7_RainSS_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 Signals has been removed from CAN FD message CLU_01_20ms in new DBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SWRCCMSS_off
+Cx1_SWRCCMSS_Key_On
+Cx2_SWRCCMSS_Reserved
+Cx3_SWRCCMSS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SWRCCSS_Idle_Position
+Cx1_SWRCCSS_Plus
+Cx2_SWRCCSS_Minus
+Cx3_SWRCCSS_Headway
+Cx4_SWRCCSS_Cancel_Pause
+Cx5_SWRCCSS_Reserved
+Cx6_SWRCCSS_Reserved
+Cx7_SWRCCSS_Reserved</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SWRCSMSS_Off
+Cx1_SWRCSMSS_Key_On
+Cx2_SWRCSMSS_Reserved
+Cx3_SWRCSMSS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLU_SWRCCrsMainSwSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLU_SWRCCrsSwSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLU_SWRCSldMainSwSta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitLength:10, Factor : 0.5,CLU_DisplaySpeedValue
+Cx3FF : Error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 Signals has been removed from CAN FD message CLU_05_00ms in new DBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 Signals has been removed from CAN FD message CLU_13_00ms in new DBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>USM_AdasDAWModNewSetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLU_AdasDAWResetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasDAWMNSR_Default
+Cx1_AdasDAWMNSR_Off
+Cx2_AdasDAWMNSR_On
+Cx3_AdasDAWMNSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasDAWRR_Default
+Cx1_AdasDAWRR_ResetReq
+Cx2_AdasDAWRR_Reserved
+Cx3_AdasDAWRR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 Signals has been removed from CAN FD message MDPS_01_10ms in new DBC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_AdasISLASR_Default
@@ -1118,81 +1205,38 @@
 Cx5_AdasISLASR_Reserved
 Cx6_AdasISLASR_Reserved
 Cx7_AdasISLASR_Invalid</t>
-  </si>
-  <si>
-    <t>CAN message added for ISLA adaptor</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>USM_AdasISLASetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>USM_AdasISLAAutoSetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_AdasISLAASR_Default
 Cx1_AdasISLAASR_Auto_Off
 Cx2_AdasISLAASR_Auto_On
 Cx3_AdasISLAASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>USM_ISLAOffstSetReq</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput SWC/VIPCDD SWC</t>
-  </si>
-  <si>
-    <t>VIPCDD SWC</t>
-  </si>
-  <si>
-    <t>Port Type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>HVIA_MDPS</t>
-  </si>
-  <si>
-    <t>HVIA_CGW</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInputAdap</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TopLevelCompostion/HkmcVehicleInput SWC</t>
-  </si>
-  <si>
-    <t>HkmcVehicleInput SWC</t>
-  </si>
-  <si>
-    <t>HSYS_CLU11</t>
-  </si>
-  <si>
-    <t>HSYS_CLU19</t>
-  </si>
-  <si>
-    <t>HSYS_MDPS12</t>
-  </si>
-  <si>
-    <t>HSYS_CGW1</t>
-  </si>
-  <si>
-    <t>HSYS_BCM_08_200ms</t>
-  </si>
-  <si>
-    <t>TopLevelCompostion</t>
-  </si>
-  <si>
-    <t>Cx0_ISLAOSR_Default
-Cx1_ISLAOSR_10kph_5mph
-Cx2_ISLAOSR_5kph_3mph
-Cx3_ISLAOSR_0
-Cx4_ISLAOSR_5kph_3mph
-Cx5_ISLAOSR_10kph_5mph
-Cx6_ISLAOSR_Reserved
-Cx7_ISLAOSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HSYS_CLU_04_00ms</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_TU_Available
+Cx1_TU_Unavailable</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum(dbc : Boolean)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1357,7 +1401,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1462,6 +1506,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1812,7 +1862,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2051,6 +2101,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -4136,10 +4190,10 @@
   <dimension ref="A1:Y93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S93" sqref="S93"/>
+      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4159,7 +4213,7 @@
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="5.875" style="26" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="40.25" style="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="79.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.625" customWidth="1"/>
     <col min="17" max="17" width="14.25" customWidth="1"/>
     <col min="18" max="18" width="15.75" customWidth="1"/>
     <col min="19" max="19" width="60.125" customWidth="1"/>
@@ -4296,7 +4350,7 @@
       <c r="R3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="S3" s="64" t="s">
+      <c r="S3" s="96" t="s">
         <v>29</v>
       </c>
       <c r="T3" s="60" t="s">
@@ -4589,10 +4643,10 @@
         <v>50</v>
       </c>
       <c r="S11" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="T11" s="73" t="s">
         <v>51</v>
-      </c>
-      <c r="T11" s="73" t="s">
-        <v>52</v>
       </c>
       <c r="U11" s="82"/>
       <c r="V11" s="41"/>
@@ -4607,16 +4661,16 @@
       <c r="N12" s="52"/>
       <c r="O12" s="87"/>
       <c r="P12" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="S12" s="55" t="s">
         <v>53</v>
-      </c>
-      <c r="Q12" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="R12" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S12" s="55" t="s">
-        <v>54</v>
       </c>
       <c r="U12" s="82"/>
     </row>
@@ -4627,16 +4681,16 @@
       <c r="N13" s="52"/>
       <c r="O13" s="87"/>
       <c r="P13" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="S13" s="55" t="s">
         <v>55</v>
-      </c>
-      <c r="Q13" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S13" s="55" t="s">
-        <v>56</v>
       </c>
       <c r="U13" s="82"/>
     </row>
@@ -4647,16 +4701,16 @@
       <c r="N14" s="52"/>
       <c r="O14" s="87"/>
       <c r="P14" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q14" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="Q14" s="68" t="s">
+      <c r="R14" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="S14" s="55" t="s">
         <v>58</v>
-      </c>
-      <c r="R14" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S14" s="55" t="s">
-        <v>59</v>
       </c>
       <c r="U14" s="82"/>
     </row>
@@ -4667,7 +4721,7 @@
       <c r="N15" s="52"/>
       <c r="O15" s="87"/>
       <c r="P15" s="61" t="s">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="Q15" s="54" t="s">
         <v>23</v>
@@ -4676,7 +4730,7 @@
         <v>50</v>
       </c>
       <c r="S15" s="55" t="s">
-        <v>61</v>
+        <v>225</v>
       </c>
       <c r="U15" s="82"/>
     </row>
@@ -4687,16 +4741,16 @@
       <c r="N16" s="52"/>
       <c r="O16" s="88"/>
       <c r="P16" s="54" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q16" s="54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="R16" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S16" s="55" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="U16" s="82"/>
     </row>
@@ -4711,10 +4765,10 @@
       <c r="M17" s="49"/>
       <c r="N17" s="52"/>
       <c r="O17" s="86" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="P17" s="61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q17" s="54" t="s">
         <v>23</v>
@@ -4723,10 +4777,10 @@
         <v>50</v>
       </c>
       <c r="S17" s="55" t="s">
-        <v>67</v>
+        <v>226</v>
       </c>
       <c r="T17" s="73" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="U17" s="82"/>
       <c r="V17" s="49"/>
@@ -4738,7 +4792,7 @@
       <c r="N18" s="52"/>
       <c r="O18" s="87"/>
       <c r="P18" s="54" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Q18" s="54" t="s">
         <v>23</v>
@@ -4747,7 +4801,7 @@
         <v>50</v>
       </c>
       <c r="S18" s="55" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="U18" s="82"/>
     </row>
@@ -4757,7 +4811,7 @@
       <c r="N19" s="52"/>
       <c r="O19" s="87"/>
       <c r="P19" s="68" t="s">
-        <v>71</v>
+        <v>227</v>
       </c>
       <c r="Q19" s="68" t="s">
         <v>23</v>
@@ -4766,10 +4820,10 @@
         <v>50</v>
       </c>
       <c r="S19" s="65" t="s">
-        <v>72</v>
+        <v>228</v>
       </c>
       <c r="T19" s="74" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="U19" s="82"/>
     </row>
@@ -4785,7 +4839,7 @@
       <c r="N20" s="52"/>
       <c r="O20" s="87"/>
       <c r="P20" s="54" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="Q20" s="54" t="s">
         <v>23</v>
@@ -4794,7 +4848,7 @@
         <v>50</v>
       </c>
       <c r="S20" s="55" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="T20" s="49"/>
       <c r="U20" s="82"/>
@@ -4807,7 +4861,7 @@
       <c r="N21" s="52"/>
       <c r="O21" s="87"/>
       <c r="P21" s="61" t="s">
-        <v>76</v>
+        <v>229</v>
       </c>
       <c r="Q21" s="54" t="s">
         <v>23</v>
@@ -4816,7 +4870,7 @@
         <v>50</v>
       </c>
       <c r="S21" s="65" t="s">
-        <v>77</v>
+        <v>230</v>
       </c>
       <c r="U21" s="82"/>
     </row>
@@ -4826,7 +4880,7 @@
       <c r="N22" s="52"/>
       <c r="O22" s="87"/>
       <c r="P22" s="54" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="Q22" s="54" t="s">
         <v>23</v>
@@ -4835,7 +4889,7 @@
         <v>50</v>
       </c>
       <c r="S22" s="55" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="U22" s="82"/>
     </row>
@@ -4851,7 +4905,7 @@
       <c r="N23" s="52"/>
       <c r="O23" s="87"/>
       <c r="P23" s="61" t="s">
-        <v>80</v>
+        <v>231</v>
       </c>
       <c r="Q23" s="54" t="s">
         <v>23</v>
@@ -4860,7 +4914,7 @@
         <v>50</v>
       </c>
       <c r="S23" s="65" t="s">
-        <v>81</v>
+        <v>232</v>
       </c>
       <c r="T23" s="49"/>
       <c r="U23" s="82"/>
@@ -4873,7 +4927,7 @@
       <c r="N24" s="52"/>
       <c r="O24" s="87"/>
       <c r="P24" s="61" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="Q24" s="54" t="s">
         <v>23</v>
@@ -4882,7 +4936,7 @@
         <v>50</v>
       </c>
       <c r="S24" s="55" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="U24" s="82"/>
     </row>
@@ -4892,7 +4946,7 @@
       <c r="N25" s="52"/>
       <c r="O25" s="87"/>
       <c r="P25" s="54" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="Q25" s="54" t="s">
         <v>23</v>
@@ -4901,7 +4955,7 @@
         <v>50</v>
       </c>
       <c r="S25" s="55" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="U25" s="82"/>
     </row>
@@ -4911,7 +4965,7 @@
       <c r="N26" s="52"/>
       <c r="O26" s="88"/>
       <c r="P26" s="54" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="Q26" s="54" t="s">
         <v>23</v>
@@ -4920,7 +4974,7 @@
         <v>50</v>
       </c>
       <c r="S26" s="55" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="U26" s="82"/>
     </row>
@@ -4935,22 +4989,22 @@
       <c r="M27" s="49"/>
       <c r="N27" s="52"/>
       <c r="O27" s="86" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="P27" s="54" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="Q27" s="68" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R27" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S27" s="55" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="T27" s="73" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="U27" s="82"/>
       <c r="V27" s="49"/>
@@ -4962,16 +5016,16 @@
       <c r="N28" s="52"/>
       <c r="O28" s="87"/>
       <c r="P28" s="61" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q28" s="54" t="s">
-        <v>23</v>
+        <v>81</v>
+      </c>
+      <c r="Q28" s="95" t="s">
+        <v>260</v>
       </c>
       <c r="R28" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S28" s="55" t="s">
-        <v>93</v>
+        <v>259</v>
       </c>
       <c r="U28" s="82"/>
     </row>
@@ -4981,7 +5035,7 @@
       <c r="N29" s="52"/>
       <c r="O29" s="87"/>
       <c r="P29" s="54" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="Q29" s="54" t="s">
         <v>23</v>
@@ -4990,7 +5044,7 @@
         <v>50</v>
       </c>
       <c r="S29" s="55" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="U29" s="82"/>
     </row>
@@ -5000,7 +5054,7 @@
       <c r="N30" s="52"/>
       <c r="O30" s="87"/>
       <c r="P30" s="54" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="Q30" s="54" t="s">
         <v>23</v>
@@ -5009,7 +5063,7 @@
         <v>50</v>
       </c>
       <c r="S30" s="55" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="U30" s="82"/>
     </row>
@@ -5019,7 +5073,7 @@
       <c r="N31" s="52"/>
       <c r="O31" s="87"/>
       <c r="P31" s="54" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="Q31" s="54" t="s">
         <v>23</v>
@@ -5028,7 +5082,7 @@
         <v>50</v>
       </c>
       <c r="S31" s="55" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="U31" s="82"/>
     </row>
@@ -5038,16 +5092,16 @@
       <c r="N32" s="52"/>
       <c r="O32" s="87"/>
       <c r="P32" s="54" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="Q32" s="54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="R32" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S32" s="55" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="U32" s="82"/>
     </row>
@@ -5057,19 +5111,19 @@
       <c r="N33" s="52"/>
       <c r="O33" s="87"/>
       <c r="P33" s="68" t="s">
-        <v>102</v>
+        <v>234</v>
       </c>
       <c r="Q33" s="68" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="R33" s="68" t="s">
         <v>50</v>
       </c>
       <c r="S33" s="65" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="T33" s="73" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="U33" s="82"/>
     </row>
@@ -5078,10 +5132,10 @@
       <c r="H34" s="51"/>
       <c r="N34" s="52"/>
       <c r="O34" s="86" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="P34" s="32" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="Q34" s="54" t="s">
         <v>23</v>
@@ -5090,7 +5144,7 @@
         <v>50</v>
       </c>
       <c r="S34" s="65" t="s">
-        <v>107</v>
+        <v>235</v>
       </c>
       <c r="T34" s="73" t="s">
         <v>37</v>
@@ -5103,7 +5157,7 @@
       <c r="N35" s="52"/>
       <c r="O35" s="87"/>
       <c r="P35" s="32" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="Q35" s="54" t="s">
         <v>23</v>
@@ -5112,10 +5166,10 @@
         <v>50</v>
       </c>
       <c r="S35" s="55" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="T35" s="73" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="U35" s="82"/>
     </row>
@@ -5125,7 +5179,7 @@
       <c r="N36" s="52"/>
       <c r="O36" s="87"/>
       <c r="P36" s="32" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="Q36" s="54" t="s">
         <v>23</v>
@@ -5134,7 +5188,7 @@
         <v>50</v>
       </c>
       <c r="S36" s="55" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="U36" s="82"/>
     </row>
@@ -5144,7 +5198,7 @@
       <c r="N37" s="52"/>
       <c r="O37" s="87"/>
       <c r="P37" s="32" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="Q37" s="54" t="s">
         <v>23</v>
@@ -5153,7 +5207,7 @@
         <v>50</v>
       </c>
       <c r="S37" s="55" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="U37" s="82"/>
     </row>
@@ -5163,7 +5217,7 @@
       <c r="N38" s="52"/>
       <c r="O38" s="87"/>
       <c r="P38" s="32" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="Q38" s="54" t="s">
         <v>23</v>
@@ -5172,7 +5226,7 @@
         <v>50</v>
       </c>
       <c r="S38" s="55" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="U38" s="82"/>
     </row>
@@ -5182,7 +5236,7 @@
       <c r="N39" s="52"/>
       <c r="O39" s="87"/>
       <c r="P39" s="32" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="Q39" s="54" t="s">
         <v>23</v>
@@ -5191,7 +5245,7 @@
         <v>50</v>
       </c>
       <c r="S39" s="55" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="U39" s="82"/>
     </row>
@@ -5201,7 +5255,7 @@
       <c r="N40" s="52"/>
       <c r="O40" s="87"/>
       <c r="P40" s="54" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="Q40" s="54" t="s">
         <v>23</v>
@@ -5210,7 +5264,7 @@
         <v>50</v>
       </c>
       <c r="S40" s="55" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="U40" s="82"/>
     </row>
@@ -5220,7 +5274,7 @@
       <c r="N41" s="52"/>
       <c r="O41" s="87"/>
       <c r="P41" s="32" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="Q41" s="54" t="s">
         <v>23</v>
@@ -5229,7 +5283,7 @@
         <v>50</v>
       </c>
       <c r="S41" s="55" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="U41" s="82"/>
     </row>
@@ -5239,7 +5293,7 @@
       <c r="N42" s="52"/>
       <c r="O42" s="87"/>
       <c r="P42" s="57" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="Q42" s="58" t="s">
         <v>23</v>
@@ -5248,7 +5302,7 @@
         <v>50</v>
       </c>
       <c r="S42" s="59" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="U42" s="82"/>
     </row>
@@ -5258,7 +5312,7 @@
       <c r="N43" s="52"/>
       <c r="O43" s="87"/>
       <c r="P43" s="69" t="s">
-        <v>125</v>
+        <v>236</v>
       </c>
       <c r="Q43" s="68" t="s">
         <v>23</v>
@@ -5267,10 +5321,10 @@
         <v>50</v>
       </c>
       <c r="S43" s="65" t="s">
-        <v>126</v>
+        <v>237</v>
       </c>
       <c r="T43" s="73" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="U43" s="82"/>
     </row>
@@ -5280,7 +5334,7 @@
       <c r="N44" s="52"/>
       <c r="O44" s="87"/>
       <c r="P44" s="32" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="Q44" s="54" t="s">
         <v>23</v>
@@ -5289,7 +5343,7 @@
         <v>50</v>
       </c>
       <c r="S44" s="55" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="U44" s="82"/>
     </row>
@@ -5299,7 +5353,7 @@
       <c r="N45" s="52"/>
       <c r="O45" s="87"/>
       <c r="P45" s="32" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="Q45" s="54" t="s">
         <v>23</v>
@@ -5308,7 +5362,7 @@
         <v>50</v>
       </c>
       <c r="S45" s="55" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="U45" s="82"/>
     </row>
@@ -5318,7 +5372,7 @@
       <c r="N46" s="52"/>
       <c r="O46" s="87"/>
       <c r="P46" s="32" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="Q46" s="54" t="s">
         <v>23</v>
@@ -5327,7 +5381,7 @@
         <v>50</v>
       </c>
       <c r="S46" s="55" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="U46" s="82"/>
     </row>
@@ -5337,7 +5391,7 @@
       <c r="N47" s="52"/>
       <c r="O47" s="87"/>
       <c r="P47" s="32" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="Q47" s="54" t="s">
         <v>23</v>
@@ -5346,7 +5400,7 @@
         <v>50</v>
       </c>
       <c r="S47" s="55" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="U47" s="82"/>
     </row>
@@ -5356,7 +5410,7 @@
       <c r="N48" s="52"/>
       <c r="O48" s="87"/>
       <c r="P48" s="32" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="Q48" s="54" t="s">
         <v>23</v>
@@ -5365,7 +5419,7 @@
         <v>50</v>
       </c>
       <c r="S48" s="55" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="U48" s="82"/>
     </row>
@@ -5375,7 +5429,7 @@
       <c r="N49" s="52"/>
       <c r="O49" s="87"/>
       <c r="P49" s="32" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="Q49" s="54" t="s">
         <v>23</v>
@@ -5384,7 +5438,7 @@
         <v>50</v>
       </c>
       <c r="S49" s="55" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="U49" s="82"/>
     </row>
@@ -5394,7 +5448,7 @@
       <c r="N50" s="52"/>
       <c r="O50" s="87"/>
       <c r="P50" s="63" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="Q50" s="54" t="s">
         <v>23</v>
@@ -5403,7 +5457,7 @@
         <v>50</v>
       </c>
       <c r="S50" s="55" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="U50" s="82"/>
     </row>
@@ -5413,7 +5467,7 @@
       <c r="N51" s="52"/>
       <c r="O51" s="87"/>
       <c r="P51" s="54" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="Q51" s="54" t="s">
         <v>23</v>
@@ -5422,7 +5476,7 @@
         <v>50</v>
       </c>
       <c r="S51" s="55" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="U51" s="82"/>
     </row>
@@ -5438,7 +5492,7 @@
       <c r="N52" s="52"/>
       <c r="O52" s="88"/>
       <c r="P52" s="57" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="Q52" s="58" t="s">
         <v>23</v>
@@ -5447,7 +5501,7 @@
         <v>50</v>
       </c>
       <c r="S52" s="59" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="T52" s="49"/>
       <c r="U52" s="82"/>
@@ -5463,7 +5517,7 @@
       <c r="M53" s="49"/>
       <c r="N53" s="52"/>
       <c r="O53" s="28" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="P53" s="33"/>
       <c r="Q53" s="29"/>
@@ -5483,22 +5537,22 @@
       <c r="M54" s="49"/>
       <c r="N54" s="52"/>
       <c r="O54" s="86" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="P54" s="54" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="Q54" s="54" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="R54" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S54" s="55" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="T54" s="73" t="s">
-        <v>151</v>
+        <v>238</v>
       </c>
       <c r="U54" s="82"/>
     </row>
@@ -5508,16 +5562,16 @@
       <c r="N55" s="52"/>
       <c r="O55" s="87"/>
       <c r="P55" s="54" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="Q55" s="54" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="R55" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S55" s="55" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="U55" s="82"/>
     </row>
@@ -5527,7 +5581,7 @@
       <c r="N56" s="52"/>
       <c r="O56" s="87"/>
       <c r="P56" s="61" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="Q56" s="54" t="s">
         <v>23</v>
@@ -5546,7 +5600,7 @@
       <c r="N57" s="52"/>
       <c r="O57" s="87"/>
       <c r="P57" s="68" t="s">
-        <v>156</v>
+        <v>242</v>
       </c>
       <c r="Q57" s="68" t="s">
         <v>23</v>
@@ -5555,10 +5609,10 @@
         <v>50</v>
       </c>
       <c r="S57" s="65" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="T57" s="73" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="U57" s="82"/>
     </row>
@@ -5568,7 +5622,7 @@
       <c r="N58" s="52"/>
       <c r="O58" s="87"/>
       <c r="P58" s="68" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="Q58" s="68" t="s">
         <v>23</v>
@@ -5577,10 +5631,10 @@
         <v>50</v>
       </c>
       <c r="S58" s="65" t="s">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="T58" s="73" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="U58" s="82"/>
     </row>
@@ -5590,7 +5644,7 @@
       <c r="N59" s="52"/>
       <c r="O59" s="87"/>
       <c r="P59" s="54" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="Q59" s="54" t="s">
         <v>23</v>
@@ -5599,7 +5653,7 @@
         <v>50</v>
       </c>
       <c r="S59" s="55" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="U59" s="82"/>
     </row>
@@ -5609,7 +5663,7 @@
       <c r="N60" s="52"/>
       <c r="O60" s="87"/>
       <c r="P60" s="68" t="s">
-        <v>163</v>
+        <v>244</v>
       </c>
       <c r="Q60" s="68" t="s">
         <v>23</v>
@@ -5618,10 +5672,10 @@
         <v>50</v>
       </c>
       <c r="S60" s="65" t="s">
-        <v>164</v>
+        <v>241</v>
       </c>
       <c r="T60" s="73" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="U60" s="82"/>
     </row>
@@ -5631,16 +5685,16 @@
       <c r="N61" s="52"/>
       <c r="O61" s="88"/>
       <c r="P61" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q61" s="54" t="s">
-        <v>149</v>
+        <v>142</v>
+      </c>
+      <c r="Q61" s="95" t="s">
+        <v>133</v>
       </c>
       <c r="R61" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S61" s="55" t="s">
-        <v>166</v>
+        <v>245</v>
       </c>
       <c r="U61" s="82"/>
     </row>
@@ -5649,10 +5703,10 @@
       <c r="H62" s="51"/>
       <c r="N62" s="52"/>
       <c r="O62" s="87" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="P62" s="61" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="Q62" s="54" t="s">
         <v>23</v>
@@ -5661,10 +5715,10 @@
         <v>50</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="T62" s="73" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="U62" s="82"/>
     </row>
@@ -5674,7 +5728,7 @@
       <c r="N63" s="52"/>
       <c r="O63" s="88"/>
       <c r="P63" s="54" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="Q63" s="54" t="s">
         <v>23</v>
@@ -5683,7 +5737,7 @@
         <v>50</v>
       </c>
       <c r="S63" s="55" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="U63" s="82"/>
     </row>
@@ -5698,22 +5752,22 @@
       <c r="M64" s="49"/>
       <c r="N64" s="52"/>
       <c r="O64" s="86" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="P64" s="54" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="Q64" s="54" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="R64" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S64" s="55" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="T64" s="73" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="U64" s="82"/>
     </row>
@@ -5723,16 +5777,16 @@
       <c r="N65" s="52"/>
       <c r="O65" s="87"/>
       <c r="P65" s="54" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="Q65" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="R65" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="S65" s="55" t="s">
         <v>153</v>
-      </c>
-      <c r="R65" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S65" s="55" t="s">
-        <v>178</v>
       </c>
       <c r="U65" s="82"/>
     </row>
@@ -5742,7 +5796,7 @@
       <c r="N66" s="52"/>
       <c r="O66" s="87"/>
       <c r="P66" s="54" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="Q66" s="54" t="s">
         <v>23</v>
@@ -5751,7 +5805,7 @@
         <v>50</v>
       </c>
       <c r="S66" s="55" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="U66" s="82"/>
     </row>
@@ -5761,7 +5815,7 @@
       <c r="N67" s="52"/>
       <c r="O67" s="87"/>
       <c r="P67" s="61" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="Q67" s="54" t="s">
         <v>23</v>
@@ -5770,7 +5824,7 @@
         <v>50</v>
       </c>
       <c r="S67" s="55" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="U67" s="82"/>
       <c r="X67" s="62"/>
@@ -5781,7 +5835,7 @@
       <c r="N68" s="52"/>
       <c r="O68" s="87"/>
       <c r="P68" s="54" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="Q68" s="54" t="s">
         <v>23</v>
@@ -5790,7 +5844,7 @@
         <v>50</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="U68" s="82"/>
     </row>
@@ -5800,7 +5854,7 @@
       <c r="N69" s="52"/>
       <c r="O69" s="87"/>
       <c r="P69" s="54" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="Q69" s="54" t="s">
         <v>23</v>
@@ -5809,7 +5863,7 @@
         <v>50</v>
       </c>
       <c r="S69" s="55" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="U69" s="82"/>
     </row>
@@ -5819,7 +5873,7 @@
       <c r="N70" s="52"/>
       <c r="O70" s="87"/>
       <c r="P70" s="54" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="Q70" s="54" t="s">
         <v>23</v>
@@ -5828,7 +5882,7 @@
         <v>50</v>
       </c>
       <c r="S70" s="55" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="U70" s="82"/>
     </row>
@@ -5838,7 +5892,7 @@
       <c r="N71" s="52"/>
       <c r="O71" s="87"/>
       <c r="P71" s="54" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="Q71" s="54" t="s">
         <v>23</v>
@@ -5847,7 +5901,7 @@
         <v>50</v>
       </c>
       <c r="S71" s="55" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="U71" s="82"/>
     </row>
@@ -5857,7 +5911,7 @@
       <c r="N72" s="52"/>
       <c r="O72" s="87"/>
       <c r="P72" s="54" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="Q72" s="54" t="s">
         <v>23</v>
@@ -5866,7 +5920,7 @@
         <v>50</v>
       </c>
       <c r="S72" s="55" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="U72" s="82"/>
     </row>
@@ -5876,7 +5930,7 @@
       <c r="N73" s="52"/>
       <c r="O73" s="87"/>
       <c r="P73" s="54" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="Q73" s="54" t="s">
         <v>23</v>
@@ -5885,7 +5939,7 @@
         <v>50</v>
       </c>
       <c r="S73" s="55" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="U73" s="82"/>
     </row>
@@ -5900,22 +5954,22 @@
       <c r="M74" s="49"/>
       <c r="N74" s="52"/>
       <c r="O74" s="86" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="P74" s="54" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="Q74" s="54" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="R74" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S74" s="55" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="T74" s="73" t="s">
-        <v>198</v>
+        <v>247</v>
       </c>
       <c r="U74" s="82"/>
       <c r="V74" s="49"/>
@@ -5928,16 +5982,16 @@
       <c r="N75" s="52"/>
       <c r="O75" s="87"/>
       <c r="P75" s="54" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="Q75" s="54" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="R75" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S75" s="55" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="U75" s="82"/>
     </row>
@@ -5947,7 +6001,7 @@
       <c r="N76" s="52"/>
       <c r="O76" s="87"/>
       <c r="P76" s="61" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="Q76" s="54" t="s">
         <v>23</v>
@@ -5956,7 +6010,7 @@
         <v>50</v>
       </c>
       <c r="S76" s="55" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="U76" s="82"/>
     </row>
@@ -5966,7 +6020,7 @@
       <c r="N77" s="52"/>
       <c r="O77" s="87"/>
       <c r="P77" s="61" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="Q77" s="54" t="s">
         <v>23</v>
@@ -5975,7 +6029,7 @@
         <v>50</v>
       </c>
       <c r="S77" s="55" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="U77" s="82"/>
     </row>
@@ -5985,7 +6039,7 @@
       <c r="N78" s="52"/>
       <c r="O78" s="87"/>
       <c r="P78" s="68" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="Q78" s="68" t="s">
         <v>23</v>
@@ -5994,10 +6048,10 @@
         <v>50</v>
       </c>
       <c r="S78" s="65" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="T78" s="73" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="U78" s="82"/>
     </row>
@@ -6007,7 +6061,7 @@
       <c r="N79" s="52"/>
       <c r="O79" s="88"/>
       <c r="P79" s="68" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="Q79" s="68" t="s">
         <v>23</v>
@@ -6016,10 +6070,10 @@
         <v>50</v>
       </c>
       <c r="S79" s="65" t="s">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="T79" s="73" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="U79" s="82"/>
     </row>
@@ -6034,22 +6088,22 @@
       <c r="M80" s="49"/>
       <c r="N80" s="52"/>
       <c r="O80" s="86" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="P80" s="54" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="Q80" s="54" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="R80" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S80" s="55" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="T80" s="73" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="U80" s="82"/>
       <c r="V80" s="49"/>
@@ -6062,16 +6116,16 @@
       <c r="N81" s="52"/>
       <c r="O81" s="87"/>
       <c r="P81" s="54" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="Q81" s="54" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="R81" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S81" s="55" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
       <c r="U81" s="82"/>
     </row>
@@ -6081,7 +6135,7 @@
       <c r="N82" s="52"/>
       <c r="O82" s="87"/>
       <c r="P82" s="54" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="Q82" s="54" t="s">
         <v>23</v>
@@ -6090,7 +6144,7 @@
         <v>50</v>
       </c>
       <c r="S82" s="55" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="U82" s="82"/>
     </row>
@@ -6100,7 +6154,7 @@
       <c r="N83" s="52"/>
       <c r="O83" s="87"/>
       <c r="P83" s="54" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="Q83" s="54" t="s">
         <v>23</v>
@@ -6109,7 +6163,7 @@
         <v>50</v>
       </c>
       <c r="S83" s="55" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
       <c r="U83" s="82"/>
     </row>
@@ -6119,7 +6173,7 @@
       <c r="N84" s="52"/>
       <c r="O84" s="87"/>
       <c r="P84" s="54" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="Q84" s="54" t="s">
         <v>23</v>
@@ -6128,7 +6182,7 @@
         <v>50</v>
       </c>
       <c r="S84" s="55" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="U84" s="82"/>
     </row>
@@ -6138,7 +6192,7 @@
       <c r="N85" s="52"/>
       <c r="O85" s="87"/>
       <c r="P85" s="61" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="Q85" s="54" t="s">
         <v>23</v>
@@ -6147,7 +6201,7 @@
         <v>50</v>
       </c>
       <c r="S85" s="55" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="U85" s="82"/>
     </row>
@@ -6157,7 +6211,7 @@
       <c r="N86" s="52"/>
       <c r="O86" s="87"/>
       <c r="P86" s="54" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="Q86" s="54" t="s">
         <v>23</v>
@@ -6166,7 +6220,7 @@
         <v>50</v>
       </c>
       <c r="S86" s="55" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="U86" s="82"/>
     </row>
@@ -6176,7 +6230,7 @@
       <c r="N87" s="52"/>
       <c r="O87" s="88"/>
       <c r="P87" s="54" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="Q87" s="54" t="s">
         <v>23</v>
@@ -6185,7 +6239,7 @@
         <v>50</v>
       </c>
       <c r="S87" s="55" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
       <c r="U87" s="82"/>
     </row>
@@ -6200,19 +6254,19 @@
       <c r="M88" s="49"/>
       <c r="N88" s="52"/>
       <c r="O88" s="86" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="P88" s="54" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="Q88" s="54" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="R88" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S88" s="55" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="T88" s="49"/>
       <c r="U88" s="82"/>
@@ -6223,16 +6277,16 @@
       <c r="N89" s="52"/>
       <c r="O89" s="87"/>
       <c r="P89" s="54" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="Q89" s="54" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="R89" s="54" t="s">
         <v>50</v>
       </c>
       <c r="S89" s="55" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="U89" s="82"/>
     </row>
@@ -6248,7 +6302,7 @@
       <c r="N90" s="52"/>
       <c r="O90" s="88"/>
       <c r="P90" s="61" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
       <c r="Q90" s="54" t="s">
         <v>23</v>
@@ -6257,7 +6311,7 @@
         <v>50</v>
       </c>
       <c r="S90" s="55" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="T90" s="49"/>
       <c r="U90" s="82"/>
@@ -6273,10 +6327,10 @@
       <c r="M91" s="41"/>
       <c r="N91" s="43"/>
       <c r="O91" s="83" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="P91" s="70" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="Q91" s="70" t="s">
         <v>23</v>
@@ -6285,10 +6339,10 @@
         <v>50</v>
       </c>
       <c r="S91" s="71" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="T91" s="75" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="U91" s="82"/>
     </row>
@@ -6304,7 +6358,7 @@
       <c r="N92" s="43"/>
       <c r="O92" s="84"/>
       <c r="P92" s="70" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="Q92" s="70" t="s">
         <v>23</v>
@@ -6313,7 +6367,7 @@
         <v>50</v>
       </c>
       <c r="S92" s="71" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="T92" s="41"/>
       <c r="U92" s="82"/>
@@ -6330,7 +6384,7 @@
       <c r="N93" s="43"/>
       <c r="O93" s="85"/>
       <c r="P93" s="70" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="Q93" s="70" t="s">
         <v>23</v>
@@ -6339,7 +6393,7 @@
         <v>50</v>
       </c>
       <c r="S93" s="71" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="T93" s="41"/>
     </row>
@@ -6415,11 +6469,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="90" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="D1" s="91"/>
       <c r="E1" s="91"/>
@@ -6429,21 +6483,21 @@
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="44" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>27</v>
@@ -6452,33 +6506,33 @@
         <v>24</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>24</v>
@@ -6486,7 +6540,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -6537,11 +6591,11 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="90" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="D1" s="91"/>
       <c r="E1" s="91"/>
@@ -6559,54 +6613,54 @@
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="44" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="I2" s="44" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="K2" s="44" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="L2" s="44" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="92" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -6622,14 +6676,14 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="93"/>
       <c r="B4" s="46" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
@@ -6644,7 +6698,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="93"/>
       <c r="B5" s="46" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>50</v>
@@ -6652,7 +6706,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -6666,7 +6720,7 @@
     <row r="6" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93"/>
       <c r="B6" s="46" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>50</v>
@@ -6675,7 +6729,7 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -6688,7 +6742,7 @@
     <row r="7" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="93"/>
       <c r="B7" s="46" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C7" s="42" t="s">
         <v>50</v>
@@ -6698,7 +6752,7 @@
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -6710,7 +6764,7 @@
     <row r="8" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="93"/>
       <c r="B8" s="46" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>50</v>
@@ -6721,7 +6775,7 @@
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
       <c r="I8" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="J8" s="43"/>
       <c r="K8" s="43"/>
@@ -6732,7 +6786,7 @@
     <row r="9" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="93"/>
       <c r="B9" s="46" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>50</v>
@@ -6744,7 +6798,7 @@
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
@@ -6754,7 +6808,7 @@
     <row r="10" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="93"/>
       <c r="B10" s="46" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>50</v>
@@ -6767,7 +6821,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
@@ -6776,7 +6830,7 @@
     <row r="11" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="93"/>
       <c r="B11" s="46" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>50</v>
@@ -6790,7 +6844,7 @@
       <c r="J11" s="43"/>
       <c r="K11" s="43"/>
       <c r="L11" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
@@ -6798,7 +6852,7 @@
     <row r="12" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="93"/>
       <c r="B12" s="46" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>50</v>
@@ -6813,14 +6867,14 @@
       <c r="K12" s="43"/>
       <c r="L12" s="43"/>
       <c r="M12" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="N12" s="43"/>
     </row>
     <row r="13" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="94"/>
       <c r="B13" s="46" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>50</v>
@@ -6836,7 +6890,7 @@
       <c r="L13" s="43"/>
       <c r="M13" s="43"/>
       <c r="N13" s="43" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -6873,12 +6927,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7087,15 +7138,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7120,18 +7183,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify mismatched signals definition between Matrix and CAN
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V2.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R2\02_SignalMatrix\HkmcVehicleInpAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB36A388-A68B-49D4-A80F-972C60B6A3C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046876FA-A2C9-4E87-9BDD-D5216CA8C1CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="262">
   <si>
     <t>Change Log</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Recreated Enum</t>
   </si>
   <si>
-    <t>HkmcVehicleInput_AdasFCASetReq</t>
-  </si>
-  <si>
     <t>Cx0_AdasFCASR_Default
 Cx1_AdasFCASR_Off
 Cx2_AdasFCASR_Warning
@@ -299,10 +296,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cx0_SldMS_Off
-Cx1_SldSMS_On</t>
-  </si>
-  <si>
     <t>CF_Clu_Vanz</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -769,16 +762,6 @@
   <si>
     <t>USM_AdasWrngTimingSetReq</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_AdasWrngTSR_Default
-Cx1_AdasWrngTSR_Late
-Cx2_AdasWrngTSR_Normal
-Cx3_AdasWrngTSR_Reserved
-Cx4_AdasWrngTSR_Reserved
-Cx5_AdasWrngTSR_Reserved
-Cx6_AdasWrngTSR_Reserved
-Cx7_AdasWrngTSR_Invalid</t>
   </si>
   <si>
     <t>USM_AdasLVDASetReq</t>
@@ -872,12 +855,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Cx0_LkaPIS_MDPS_Not_Plugged
-Cx1_LkaPIS_MDPS_Plugged_In
-Cx2_LkaPIS_Not_Used
-Cx3_LkaPIS_Error_Indicator</t>
-  </si>
-  <si>
     <t>MDPS_LkaToiActvSta</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -909,10 +886,6 @@
   <si>
     <t>MDPS_StrTqSnsrVal</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cx0_StrTSV_Not_Used
-Cx1_StrTSV_Error_Indicator</t>
   </si>
   <si>
     <t>HSYS_BCM_08_200ms</t>
@@ -1237,6 +1210,42 @@
   </si>
   <si>
     <t>enum(dbc : Boolean)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasWrngTSR_Default
+Cx1_AdasWrngTSR_Late
+Cx2_AdasWrngTSR_Normal
+Cx3_AdasWrngTSR_Reserved
+Cx4_AdasWrngTSR_Reserved
+Cx5_AdasWrngTSR_Reserved
+Cx6_AdasWrngTSR_Reserved
+Cx7_AdasWrngTSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaPIS_MDPS_Not_Plugged
+Cx1_LkaPIS_MDPS_Plugged_In
+Cx2_LkaPIS_Not_Used
+Cx3_LkaPIS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_StrTSV_Not_Used
+Cx1_StrTSV_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum(dbc : uint16)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcVehicleInput_AdasFCASetReq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_SldMS_Off
+Cx1_SldSMS_On</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1862,7 +1871,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2104,6 +2113,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4190,10 +4202,10 @@
   <dimension ref="A1:Y93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4383,7 +4395,7 @@
         <v>27</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>31</v>
+        <v>260</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>23</v>
@@ -4392,7 +4404,7 @@
         <v>24</v>
       </c>
       <c r="S4" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="T4" s="41"/>
       <c r="U4" s="82"/>
@@ -4422,7 +4434,7 @@
         <v>21</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q5" s="40" t="s">
         <v>23</v>
@@ -4431,7 +4443,7 @@
         <v>24</v>
       </c>
       <c r="S5" s="53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T5" s="41"/>
       <c r="U5" s="82"/>
@@ -4461,7 +4473,7 @@
         <v>27</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="40" t="s">
         <v>23</v>
@@ -4470,10 +4482,10 @@
         <v>24</v>
       </c>
       <c r="S6" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="T6" s="60" t="s">
         <v>36</v>
-      </c>
-      <c r="T6" s="60" t="s">
-        <v>37</v>
       </c>
       <c r="U6" s="82"/>
       <c r="V6" s="41"/>
@@ -4492,7 +4504,7 @@
         <v>27</v>
       </c>
       <c r="P7" s="66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="66" t="s">
         <v>23</v>
@@ -4501,10 +4513,10 @@
         <v>24</v>
       </c>
       <c r="S7" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="67" t="s">
         <v>39</v>
-      </c>
-      <c r="T7" s="67" t="s">
-        <v>40</v>
       </c>
       <c r="U7" s="82"/>
     </row>
@@ -4526,10 +4538,10 @@
         <v>7</v>
       </c>
       <c r="O8" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="40" t="s">
         <v>41</v>
-      </c>
-      <c r="P8" s="40" t="s">
-        <v>42</v>
       </c>
       <c r="Q8" s="40" t="s">
         <v>23</v>
@@ -4538,7 +4550,7 @@
         <v>24</v>
       </c>
       <c r="S8" s="53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T8" s="41"/>
       <c r="U8" s="82"/>
@@ -4565,10 +4577,10 @@
         <v>8</v>
       </c>
       <c r="O9" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="40" t="s">
         <v>44</v>
-      </c>
-      <c r="P9" s="40" t="s">
-        <v>45</v>
       </c>
       <c r="Q9" s="40" t="s">
         <v>23</v>
@@ -4577,7 +4589,7 @@
         <v>24</v>
       </c>
       <c r="S9" s="53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T9" s="41"/>
       <c r="U9" s="82"/>
@@ -4602,7 +4614,7 @@
       <c r="M10" s="49"/>
       <c r="N10" s="52"/>
       <c r="O10" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -4631,22 +4643,22 @@
       <c r="M11" s="49"/>
       <c r="N11" s="52"/>
       <c r="O11" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="54" t="s">
         <v>48</v>
-      </c>
-      <c r="P11" s="54" t="s">
-        <v>49</v>
       </c>
       <c r="Q11" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R11" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S11" s="55" t="s">
+        <v>218</v>
+      </c>
+      <c r="T11" s="73" t="s">
         <v>50</v>
-      </c>
-      <c r="S11" s="55" t="s">
-        <v>223</v>
-      </c>
-      <c r="T11" s="73" t="s">
-        <v>51</v>
       </c>
       <c r="U11" s="82"/>
       <c r="V11" s="41"/>
@@ -4661,16 +4673,16 @@
       <c r="N12" s="52"/>
       <c r="O12" s="87"/>
       <c r="P12" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q12" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R12" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S12" s="55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U12" s="82"/>
     </row>
@@ -4681,16 +4693,16 @@
       <c r="N13" s="52"/>
       <c r="O13" s="87"/>
       <c r="P13" s="54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q13" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R13" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S13" s="55" t="s">
-        <v>55</v>
+        <v>261</v>
       </c>
       <c r="U13" s="82"/>
     </row>
@@ -4701,16 +4713,16 @@
       <c r="N14" s="52"/>
       <c r="O14" s="87"/>
       <c r="P14" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S14" s="55" t="s">
         <v>56</v>
-      </c>
-      <c r="Q14" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="R14" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S14" s="55" t="s">
-        <v>58</v>
       </c>
       <c r="U14" s="82"/>
     </row>
@@ -4721,16 +4733,16 @@
       <c r="N15" s="52"/>
       <c r="O15" s="87"/>
       <c r="P15" s="61" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="Q15" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R15" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S15" s="55" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="U15" s="82"/>
     </row>
@@ -4741,16 +4753,16 @@
       <c r="N16" s="52"/>
       <c r="O16" s="88"/>
       <c r="P16" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="R16" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S16" s="55" t="s">
         <v>59</v>
-      </c>
-      <c r="Q16" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="R16" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S16" s="55" t="s">
-        <v>61</v>
       </c>
       <c r="U16" s="82"/>
     </row>
@@ -4765,22 +4777,22 @@
       <c r="M17" s="49"/>
       <c r="N17" s="52"/>
       <c r="O17" s="86" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P17" s="61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q17" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R17" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S17" s="55" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="T17" s="73" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="U17" s="82"/>
       <c r="V17" s="49"/>
@@ -4792,16 +4804,16 @@
       <c r="N18" s="52"/>
       <c r="O18" s="87"/>
       <c r="P18" s="54" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q18" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R18" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S18" s="55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U18" s="82"/>
     </row>
@@ -4811,19 +4823,19 @@
       <c r="N19" s="52"/>
       <c r="O19" s="87"/>
       <c r="P19" s="68" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="Q19" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R19" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S19" s="65" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="T19" s="74" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U19" s="82"/>
     </row>
@@ -4839,16 +4851,16 @@
       <c r="N20" s="52"/>
       <c r="O20" s="87"/>
       <c r="P20" s="54" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q20" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R20" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S20" s="55" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="T20" s="49"/>
       <c r="U20" s="82"/>
@@ -4861,16 +4873,16 @@
       <c r="N21" s="52"/>
       <c r="O21" s="87"/>
       <c r="P21" s="61" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Q21" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R21" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S21" s="65" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="U21" s="82"/>
     </row>
@@ -4880,16 +4892,16 @@
       <c r="N22" s="52"/>
       <c r="O22" s="87"/>
       <c r="P22" s="54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q22" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R22" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S22" s="55" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U22" s="82"/>
     </row>
@@ -4905,16 +4917,16 @@
       <c r="N23" s="52"/>
       <c r="O23" s="87"/>
       <c r="P23" s="61" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="Q23" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R23" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S23" s="65" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="T23" s="49"/>
       <c r="U23" s="82"/>
@@ -4927,16 +4939,16 @@
       <c r="N24" s="52"/>
       <c r="O24" s="87"/>
       <c r="P24" s="61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q24" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R24" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S24" s="55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="U24" s="82"/>
     </row>
@@ -4946,16 +4958,16 @@
       <c r="N25" s="52"/>
       <c r="O25" s="87"/>
       <c r="P25" s="54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="Q25" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R25" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S25" s="55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="U25" s="82"/>
     </row>
@@ -4965,16 +4977,16 @@
       <c r="N26" s="52"/>
       <c r="O26" s="88"/>
       <c r="P26" s="54" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q26" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R26" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S26" s="55" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="U26" s="82"/>
     </row>
@@ -4989,22 +5001,22 @@
       <c r="M27" s="49"/>
       <c r="N27" s="52"/>
       <c r="O27" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="P27" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q27" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="R27" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S27" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="P27" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q27" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="R27" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S27" s="55" t="s">
-        <v>80</v>
-      </c>
       <c r="T27" s="73" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="U27" s="82"/>
       <c r="V27" s="49"/>
@@ -5016,16 +5028,16 @@
       <c r="N28" s="52"/>
       <c r="O28" s="87"/>
       <c r="P28" s="61" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q28" s="95" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="R28" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S28" s="55" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="U28" s="82"/>
     </row>
@@ -5035,16 +5047,16 @@
       <c r="N29" s="52"/>
       <c r="O29" s="87"/>
       <c r="P29" s="54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q29" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R29" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S29" s="55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="U29" s="82"/>
     </row>
@@ -5054,16 +5066,16 @@
       <c r="N30" s="52"/>
       <c r="O30" s="87"/>
       <c r="P30" s="54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q30" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R30" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S30" s="55" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="U30" s="82"/>
     </row>
@@ -5073,16 +5085,16 @@
       <c r="N31" s="52"/>
       <c r="O31" s="87"/>
       <c r="P31" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q31" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R31" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S31" s="55" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="U31" s="82"/>
     </row>
@@ -5092,16 +5104,16 @@
       <c r="N32" s="52"/>
       <c r="O32" s="87"/>
       <c r="P32" s="54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q32" s="54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R32" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S32" s="55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="U32" s="82"/>
     </row>
@@ -5111,19 +5123,19 @@
       <c r="N33" s="52"/>
       <c r="O33" s="87"/>
       <c r="P33" s="68" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="Q33" s="68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R33" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S33" s="65" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T33" s="73" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U33" s="82"/>
     </row>
@@ -5132,22 +5144,22 @@
       <c r="H34" s="51"/>
       <c r="N34" s="52"/>
       <c r="O34" s="86" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P34" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q34" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R34" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S34" s="65" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="T34" s="73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U34" s="82"/>
     </row>
@@ -5157,19 +5169,19 @@
       <c r="N35" s="52"/>
       <c r="O35" s="87"/>
       <c r="P35" s="32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q35" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R35" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S35" s="55" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T35" s="73" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U35" s="82"/>
     </row>
@@ -5179,16 +5191,16 @@
       <c r="N36" s="52"/>
       <c r="O36" s="87"/>
       <c r="P36" s="32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q36" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R36" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S36" s="55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U36" s="82"/>
     </row>
@@ -5198,16 +5210,16 @@
       <c r="N37" s="52"/>
       <c r="O37" s="87"/>
       <c r="P37" s="32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q37" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R37" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S37" s="55" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="U37" s="82"/>
     </row>
@@ -5217,16 +5229,16 @@
       <c r="N38" s="52"/>
       <c r="O38" s="87"/>
       <c r="P38" s="32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q38" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R38" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S38" s="55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="U38" s="82"/>
     </row>
@@ -5236,16 +5248,16 @@
       <c r="N39" s="52"/>
       <c r="O39" s="87"/>
       <c r="P39" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q39" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R39" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S39" s="55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U39" s="82"/>
     </row>
@@ -5255,16 +5267,16 @@
       <c r="N40" s="52"/>
       <c r="O40" s="87"/>
       <c r="P40" s="54" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Q40" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R40" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S40" s="55" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U40" s="82"/>
     </row>
@@ -5274,16 +5286,16 @@
       <c r="N41" s="52"/>
       <c r="O41" s="87"/>
       <c r="P41" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q41" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R41" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S41" s="55" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="U41" s="82"/>
     </row>
@@ -5293,16 +5305,16 @@
       <c r="N42" s="52"/>
       <c r="O42" s="87"/>
       <c r="P42" s="57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="Q42" s="58" t="s">
         <v>23</v>
       </c>
       <c r="R42" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S42" s="59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U42" s="82"/>
     </row>
@@ -5312,19 +5324,19 @@
       <c r="N43" s="52"/>
       <c r="O43" s="87"/>
       <c r="P43" s="69" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="Q43" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R43" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S43" s="65" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="T43" s="73" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="U43" s="82"/>
     </row>
@@ -5334,16 +5346,16 @@
       <c r="N44" s="52"/>
       <c r="O44" s="87"/>
       <c r="P44" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Q44" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R44" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S44" s="55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U44" s="82"/>
     </row>
@@ -5353,16 +5365,16 @@
       <c r="N45" s="52"/>
       <c r="O45" s="87"/>
       <c r="P45" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q45" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R45" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S45" s="55" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U45" s="82"/>
     </row>
@@ -5372,16 +5384,16 @@
       <c r="N46" s="52"/>
       <c r="O46" s="87"/>
       <c r="P46" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q46" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R46" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S46" s="55" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U46" s="82"/>
     </row>
@@ -5391,16 +5403,16 @@
       <c r="N47" s="52"/>
       <c r="O47" s="87"/>
       <c r="P47" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q47" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R47" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S47" s="55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="U47" s="82"/>
     </row>
@@ -5410,16 +5422,16 @@
       <c r="N48" s="52"/>
       <c r="O48" s="87"/>
       <c r="P48" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q48" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R48" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S48" s="55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="U48" s="82"/>
     </row>
@@ -5429,16 +5441,16 @@
       <c r="N49" s="52"/>
       <c r="O49" s="87"/>
       <c r="P49" s="32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q49" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R49" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S49" s="55" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="U49" s="82"/>
     </row>
@@ -5448,16 +5460,16 @@
       <c r="N50" s="52"/>
       <c r="O50" s="87"/>
       <c r="P50" s="63" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q50" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R50" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S50" s="55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U50" s="82"/>
     </row>
@@ -5467,16 +5479,16 @@
       <c r="N51" s="52"/>
       <c r="O51" s="87"/>
       <c r="P51" s="54" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="Q51" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R51" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S51" s="55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U51" s="82"/>
     </row>
@@ -5492,16 +5504,16 @@
       <c r="N52" s="52"/>
       <c r="O52" s="88"/>
       <c r="P52" s="57" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="Q52" s="58" t="s">
         <v>23</v>
       </c>
       <c r="R52" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S52" s="59" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T52" s="49"/>
       <c r="U52" s="82"/>
@@ -5517,7 +5529,7 @@
       <c r="M53" s="49"/>
       <c r="N53" s="52"/>
       <c r="O53" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P53" s="33"/>
       <c r="Q53" s="29"/>
@@ -5537,22 +5549,22 @@
       <c r="M54" s="49"/>
       <c r="N54" s="52"/>
       <c r="O54" s="86" t="s">
+        <v>129</v>
+      </c>
+      <c r="P54" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q54" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="P54" s="54" t="s">
+      <c r="R54" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S54" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="Q54" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="R54" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S54" s="55" t="s">
-        <v>134</v>
-      </c>
       <c r="T54" s="73" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="U54" s="82"/>
     </row>
@@ -5562,16 +5574,16 @@
       <c r="N55" s="52"/>
       <c r="O55" s="87"/>
       <c r="P55" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q55" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="R55" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S55" s="55" t="s">
         <v>135</v>
-      </c>
-      <c r="Q55" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="R55" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S55" s="55" t="s">
-        <v>137</v>
       </c>
       <c r="U55" s="82"/>
     </row>
@@ -5581,13 +5593,13 @@
       <c r="N56" s="52"/>
       <c r="O56" s="87"/>
       <c r="P56" s="61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="Q56" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R56" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S56" s="55" t="s">
         <v>25</v>
@@ -5600,19 +5612,19 @@
       <c r="N57" s="52"/>
       <c r="O57" s="87"/>
       <c r="P57" s="68" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="Q57" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R57" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S57" s="65" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="T57" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="U57" s="82"/>
     </row>
@@ -5622,19 +5634,19 @@
       <c r="N58" s="52"/>
       <c r="O58" s="87"/>
       <c r="P58" s="68" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="Q58" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R58" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S58" s="65" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="T58" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="U58" s="82"/>
     </row>
@@ -5644,16 +5656,16 @@
       <c r="N59" s="52"/>
       <c r="O59" s="87"/>
       <c r="P59" s="54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q59" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R59" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S59" s="55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U59" s="82"/>
     </row>
@@ -5663,19 +5675,19 @@
       <c r="N60" s="52"/>
       <c r="O60" s="87"/>
       <c r="P60" s="68" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="Q60" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R60" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S60" s="65" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="T60" s="73" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="U60" s="82"/>
     </row>
@@ -5685,16 +5697,16 @@
       <c r="N61" s="52"/>
       <c r="O61" s="88"/>
       <c r="P61" s="54" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q61" s="95" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R61" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S61" s="55" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="U61" s="82"/>
     </row>
@@ -5703,22 +5715,22 @@
       <c r="H62" s="51"/>
       <c r="N62" s="52"/>
       <c r="O62" s="87" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P62" s="61" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q62" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R62" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T62" s="73" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="U62" s="82"/>
     </row>
@@ -5728,16 +5740,16 @@
       <c r="N63" s="52"/>
       <c r="O63" s="88"/>
       <c r="P63" s="54" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="Q63" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R63" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S63" s="55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="U63" s="82"/>
     </row>
@@ -5752,22 +5764,22 @@
       <c r="M64" s="49"/>
       <c r="N64" s="52"/>
       <c r="O64" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="P64" s="54" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q64" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="R64" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="S64" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="P64" s="54" t="s">
+      <c r="T64" s="73" t="s">
         <v>149</v>
-      </c>
-      <c r="Q64" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="R64" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S64" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="T64" s="73" t="s">
-        <v>151</v>
       </c>
       <c r="U64" s="82"/>
     </row>
@@ -5777,16 +5789,16 @@
       <c r="N65" s="52"/>
       <c r="O65" s="87"/>
       <c r="P65" s="54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q65" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R65" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S65" s="55" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U65" s="82"/>
     </row>
@@ -5796,16 +5808,16 @@
       <c r="N66" s="52"/>
       <c r="O66" s="87"/>
       <c r="P66" s="54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q66" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R66" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S66" s="55" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="U66" s="82"/>
     </row>
@@ -5815,16 +5827,16 @@
       <c r="N67" s="52"/>
       <c r="O67" s="87"/>
       <c r="P67" s="61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q67" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R67" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S67" s="55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="U67" s="82"/>
       <c r="X67" s="62"/>
@@ -5835,16 +5847,16 @@
       <c r="N68" s="52"/>
       <c r="O68" s="87"/>
       <c r="P68" s="54" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q68" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R68" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="U68" s="82"/>
     </row>
@@ -5854,16 +5866,16 @@
       <c r="N69" s="52"/>
       <c r="O69" s="87"/>
       <c r="P69" s="54" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q69" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R69" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S69" s="55" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="U69" s="82"/>
     </row>
@@ -5873,16 +5885,16 @@
       <c r="N70" s="52"/>
       <c r="O70" s="87"/>
       <c r="P70" s="54" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q70" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R70" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S70" s="55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="U70" s="82"/>
     </row>
@@ -5892,16 +5904,16 @@
       <c r="N71" s="52"/>
       <c r="O71" s="87"/>
       <c r="P71" s="54" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q71" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R71" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S71" s="55" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="U71" s="82"/>
     </row>
@@ -5911,16 +5923,16 @@
       <c r="N72" s="52"/>
       <c r="O72" s="87"/>
       <c r="P72" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q72" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R72" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S72" s="55" t="s">
-        <v>167</v>
+        <v>256</v>
       </c>
       <c r="U72" s="82"/>
     </row>
@@ -5930,16 +5942,16 @@
       <c r="N73" s="52"/>
       <c r="O73" s="87"/>
       <c r="P73" s="54" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="Q73" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R73" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S73" s="55" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="U73" s="82"/>
     </row>
@@ -5954,22 +5966,22 @@
       <c r="M74" s="49"/>
       <c r="N74" s="52"/>
       <c r="O74" s="86" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="P74" s="54" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Q74" s="54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R74" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S74" s="55" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="T74" s="73" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="U74" s="82"/>
       <c r="V74" s="49"/>
@@ -5982,16 +5994,16 @@
       <c r="N75" s="52"/>
       <c r="O75" s="87"/>
       <c r="P75" s="54" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q75" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R75" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S75" s="55" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="U75" s="82"/>
     </row>
@@ -6001,16 +6013,16 @@
       <c r="N76" s="52"/>
       <c r="O76" s="87"/>
       <c r="P76" s="61" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q76" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R76" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S76" s="55" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="U76" s="82"/>
     </row>
@@ -6020,16 +6032,16 @@
       <c r="N77" s="52"/>
       <c r="O77" s="87"/>
       <c r="P77" s="61" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q77" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R77" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S77" s="55" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="U77" s="82"/>
     </row>
@@ -6039,19 +6051,19 @@
       <c r="N78" s="52"/>
       <c r="O78" s="87"/>
       <c r="P78" s="68" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="Q78" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R78" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S78" s="65" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="T78" s="73" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U78" s="82"/>
     </row>
@@ -6061,19 +6073,19 @@
       <c r="N79" s="52"/>
       <c r="O79" s="88"/>
       <c r="P79" s="68" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="Q79" s="68" t="s">
         <v>23</v>
       </c>
       <c r="R79" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S79" s="65" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="T79" s="73" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="U79" s="82"/>
     </row>
@@ -6088,22 +6100,22 @@
       <c r="M80" s="49"/>
       <c r="N80" s="52"/>
       <c r="O80" s="86" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="P80" s="54" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q80" s="54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="R80" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S80" s="55" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T80" s="73" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="U80" s="82"/>
       <c r="V80" s="49"/>
@@ -6116,16 +6128,16 @@
       <c r="N81" s="52"/>
       <c r="O81" s="87"/>
       <c r="P81" s="54" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Q81" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R81" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S81" s="55" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="U81" s="82"/>
     </row>
@@ -6135,16 +6147,16 @@
       <c r="N82" s="52"/>
       <c r="O82" s="87"/>
       <c r="P82" s="54" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q82" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R82" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S82" s="55" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="U82" s="82"/>
     </row>
@@ -6154,16 +6166,16 @@
       <c r="N83" s="52"/>
       <c r="O83" s="87"/>
       <c r="P83" s="54" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q83" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R83" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S83" s="55" t="s">
-        <v>188</v>
+        <v>257</v>
       </c>
       <c r="U83" s="82"/>
     </row>
@@ -6173,16 +6185,16 @@
       <c r="N84" s="52"/>
       <c r="O84" s="87"/>
       <c r="P84" s="54" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="Q84" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R84" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S84" s="55" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="U84" s="82"/>
     </row>
@@ -6192,16 +6204,16 @@
       <c r="N85" s="52"/>
       <c r="O85" s="87"/>
       <c r="P85" s="61" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="Q85" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R85" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S85" s="55" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U85" s="82"/>
     </row>
@@ -6211,16 +6223,16 @@
       <c r="N86" s="52"/>
       <c r="O86" s="87"/>
       <c r="P86" s="54" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="Q86" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R86" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S86" s="55" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="U86" s="82"/>
     </row>
@@ -6229,17 +6241,17 @@
       <c r="H87" s="51"/>
       <c r="N87" s="52"/>
       <c r="O87" s="88"/>
-      <c r="P87" s="54" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q87" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="R87" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="S87" s="55" t="s">
-        <v>196</v>
+      <c r="P87" s="95" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q87" s="95" t="s">
+        <v>259</v>
+      </c>
+      <c r="R87" s="95" t="s">
+        <v>49</v>
+      </c>
+      <c r="S87" s="97" t="s">
+        <v>258</v>
       </c>
       <c r="U87" s="82"/>
     </row>
@@ -6254,19 +6266,19 @@
       <c r="M88" s="49"/>
       <c r="N88" s="52"/>
       <c r="O88" s="86" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P88" s="54" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="Q88" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R88" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S88" s="55" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="T88" s="49"/>
       <c r="U88" s="82"/>
@@ -6277,16 +6289,16 @@
       <c r="N89" s="52"/>
       <c r="O89" s="87"/>
       <c r="P89" s="54" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="Q89" s="54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R89" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S89" s="55" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="U89" s="82"/>
     </row>
@@ -6302,16 +6314,16 @@
       <c r="N90" s="52"/>
       <c r="O90" s="88"/>
       <c r="P90" s="61" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Q90" s="54" t="s">
         <v>23</v>
       </c>
       <c r="R90" s="54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S90" s="55" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="T90" s="49"/>
       <c r="U90" s="82"/>
@@ -6327,22 +6339,22 @@
       <c r="M91" s="41"/>
       <c r="N91" s="43"/>
       <c r="O91" s="83" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="P91" s="70" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="Q91" s="70" t="s">
         <v>23</v>
       </c>
       <c r="R91" s="70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S91" s="71" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="T91" s="75" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="U91" s="82"/>
     </row>
@@ -6358,16 +6370,16 @@
       <c r="N92" s="43"/>
       <c r="O92" s="84"/>
       <c r="P92" s="70" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="Q92" s="70" t="s">
         <v>23</v>
       </c>
       <c r="R92" s="70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S92" s="71" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="T92" s="41"/>
       <c r="U92" s="82"/>
@@ -6384,16 +6396,16 @@
       <c r="N93" s="43"/>
       <c r="O93" s="85"/>
       <c r="P93" s="70" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="Q93" s="70" t="s">
         <v>23</v>
       </c>
       <c r="R93" s="70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S93" s="71" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="T93" s="41"/>
     </row>
@@ -6469,11 +6481,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="90" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D1" s="91"/>
       <c r="E1" s="91"/>
@@ -6483,21 +6495,21 @@
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="44" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>27</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>27</v>
@@ -6506,33 +6518,33 @@
         <v>24</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>24</v>
@@ -6540,7 +6552,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -6591,11 +6603,11 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="89" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="90" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D1" s="91"/>
       <c r="E1" s="91"/>
@@ -6613,54 +6625,54 @@
       <c r="A2" s="89"/>
       <c r="B2" s="89"/>
       <c r="C2" s="44" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I2" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K2" s="44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L2" s="44" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="92" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -6676,14 +6688,14 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="93"/>
       <c r="B4" s="46" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
@@ -6698,15 +6710,15 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="93"/>
       <c r="B5" s="46" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -6720,16 +6732,16 @@
     <row r="6" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93"/>
       <c r="B6" s="46" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -6742,17 +6754,17 @@
     <row r="7" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="93"/>
       <c r="B7" s="46" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -6764,10 +6776,10 @@
     <row r="8" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="93"/>
       <c r="B8" s="46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -6775,7 +6787,7 @@
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
       <c r="I8" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J8" s="43"/>
       <c r="K8" s="43"/>
@@ -6786,10 +6798,10 @@
     <row r="9" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="93"/>
       <c r="B9" s="46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -6798,7 +6810,7 @@
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
@@ -6808,10 +6820,10 @@
     <row r="10" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="93"/>
       <c r="B10" s="46" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -6821,7 +6833,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
@@ -6830,10 +6842,10 @@
     <row r="11" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="93"/>
       <c r="B11" s="46" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
@@ -6844,7 +6856,7 @@
       <c r="J11" s="43"/>
       <c r="K11" s="43"/>
       <c r="L11" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
@@ -6852,10 +6864,10 @@
     <row r="12" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="93"/>
       <c r="B12" s="46" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -6867,17 +6879,17 @@
       <c r="K12" s="43"/>
       <c r="L12" s="43"/>
       <c r="M12" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="N12" s="43"/>
     </row>
     <row r="13" spans="1:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="94"/>
       <c r="B13" s="46" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -6890,7 +6902,7 @@
       <c r="L13" s="43"/>
       <c r="M13" s="43"/>
       <c r="N13" s="43" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>